<commit_message>
finished draft of follow set
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35560" windowHeight="31560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
-    <sheet name="f&amp;F" sheetId="2" r:id="rId2"/>
+    <sheet name="firsts" sheetId="2" r:id="rId2"/>
+    <sheet name="Follows" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="1">'f&amp;F'!$A$2:$K$74</definedName>
+    <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="1">firsts!$A$2:$J$74</definedName>
+    <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="2">Follows!$A$2:$G$42</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="113">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -217,6 +219,9 @@
     <t>VARIABLE</t>
   </si>
   <si>
+    <t>assignop</t>
+  </si>
+  <si>
     <t>EXPRESSION</t>
   </si>
   <si>
@@ -328,9 +333,6 @@
     <t>Subprod</t>
   </si>
   <si>
-    <t>follows</t>
-  </si>
-  <si>
     <t>id num ( not</t>
   </si>
   <si>
@@ -344,6 +346,45 @@
   </si>
   <si>
     <t>id call begin if while</t>
+  </si>
+  <si>
+    <t>IDENTIFIER_LIST'</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>procedure, begin</t>
+  </si>
+  <si>
+    <t>; F(PARAMATER_LIST')</t>
+  </si>
+  <si>
+    <t>Follows</t>
+  </si>
+  <si>
+    <t>F(TYPE)</t>
+  </si>
+  <si>
+    <t>var procedure begin</t>
+  </si>
+  <si>
+    <t>. ;</t>
+  </si>
+  <si>
+    <t>; end else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">) </t>
+  </si>
+  <si>
+    <t>; end else then do ] , )</t>
+  </si>
+  <si>
+    <t>relop ; end else then do ] , )</t>
+  </si>
+  <si>
+    <t>addop relop ; end else then do ] , )</t>
   </si>
 </sst>
 </file>
@@ -408,8 +449,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -433,7 +514,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -441,6 +522,26 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +549,26 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,6 +577,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -831,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A41" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -844,30 +969,26 @@
     <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="26" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="26" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -884,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -901,7 +1022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -918,7 +1039,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -935,7 +1056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -952,7 +1073,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -969,7 +1090,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -986,7 +1107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1003,7 +1124,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1020,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1158,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1054,7 +1175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1071,7 +1192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1088,7 +1209,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1105,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1561,7 +1682,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1595,7 +1716,7 @@
         <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1612,7 +1733,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1623,13 +1744,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1640,7 +1761,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -1651,7 +1772,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -1668,13 +1789,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -1685,13 +1806,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
@@ -1702,30 +1823,30 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D52" t="s">
         <v>10</v>
@@ -1736,13 +1857,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
@@ -1753,13 +1874,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
@@ -1770,13 +1891,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
@@ -1787,13 +1908,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
@@ -1804,13 +1925,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -1821,30 +1942,30 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
       </c>
       <c r="E58" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -1855,13 +1976,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
@@ -1872,13 +1993,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -1889,30 +2010,30 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D62" t="s">
         <v>10</v>
       </c>
       <c r="E62" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
@@ -1923,13 +2044,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
         <v>10</v>
@@ -1940,30 +2061,30 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D65" t="s">
         <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D66" t="s">
         <v>10</v>
@@ -1974,13 +2095,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D67" t="s">
         <v>10</v>
@@ -1991,13 +2112,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
@@ -2008,13 +2129,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -2025,30 +2146,30 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D70" t="s">
         <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
@@ -2059,13 +2180,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
@@ -2076,36 +2197,527 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
       <c r="C74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="26" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
         <v>77</v>
       </c>
-      <c r="D74" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" t="s">
-        <v>89</v>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix in follow set
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="112">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -357,15 +357,9 @@
     <t>procedure, begin</t>
   </si>
   <si>
-    <t>; F(PARAMATER_LIST')</t>
-  </si>
-  <si>
     <t>Follows</t>
   </si>
   <si>
-    <t>F(TYPE)</t>
-  </si>
-  <si>
     <t>var procedure begin</t>
   </si>
   <si>
@@ -385,6 +379,9 @@
   </si>
   <si>
     <t>addop relop ; end else then do ] , )</t>
+  </si>
+  <si>
+    <t>; )</t>
   </si>
 </sst>
 </file>
@@ -449,8 +446,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -514,7 +513,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -542,6 +541,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -569,6 +569,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
@@ -2244,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2266,7 +2267,7 @@
         <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2354,7 +2355,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2365,7 +2366,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2431,7 +2432,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2442,7 +2443,7 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2486,7 +2487,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2497,7 +2498,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2541,7 +2542,7 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2552,7 +2553,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2585,7 +2586,7 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2596,7 +2597,7 @@
         <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2607,7 +2608,7 @@
         <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2629,7 +2630,7 @@
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2640,7 +2641,7 @@
         <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2651,7 +2652,7 @@
         <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2662,7 +2663,7 @@
         <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2673,7 +2674,7 @@
         <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2684,7 +2685,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3">

</xml_diff>

<commit_message>
another fix in follow set
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="113">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>; )</t>
+  </si>
+  <si>
+    <t>addop relop ; end else then do ] , ) mulop</t>
   </si>
 </sst>
 </file>
@@ -446,8 +449,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,7 +520,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -542,6 +549,8 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -570,6 +579,8 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -960,7 +971,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2245,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2695,8 +2706,8 @@
       <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>95</v>
+      <c r="C40" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2706,8 +2717,8 @@
       <c r="B41" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>95</v>
+      <c r="C41" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3">

</xml_diff>

<commit_message>
started on parse table
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,16 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17500" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="17720" yWindow="0" windowWidth="11080" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
     <sheet name="firsts" sheetId="2" r:id="rId2"/>
     <sheet name="Follows" sheetId="4" r:id="rId3"/>
+    <sheet name="G" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="1">firsts!$A$2:$J$74</definedName>
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="2">Follows!$A$2:$G$42</definedName>
+    <definedName name="copyForImport" localSheetId="3">G!$A$1:$B$73</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -42,11 +45,28 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="ENTERPRISE:Users:kuxhausen:Desktop:compiler-front-end:doc:2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" tab="0" qualifier="none" delimiter="-">
+      <textFields count="3">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="copyForImport" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="ENTERPRISE:Users:kuxhausen:Desktop:compiler-front-end:doc:copyForImport" tab="0" qualifier="none" delimiter="@">
+      <textFields count="2">
+        <textField type="text"/>
+        <textField type="text"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="227">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -354,9 +374,6 @@
     <t>$</t>
   </si>
   <si>
-    <t>procedure, begin</t>
-  </si>
-  <si>
     <t>Follows</t>
   </si>
   <si>
@@ -385,13 +402,358 @@
   </si>
   <si>
     <t>addop relop ; end else then do ] , ) mulop</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>procedure begin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 PROGRAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 PROGRAM^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 PROGRAM^^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 IDENTIFIER_LIST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 IDENTIFIER_LIST` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 DECLARATIONS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 DECLARATIONS` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 TYPE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 STANDARD_TYPE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 SUBPROGRAM_DECLARATIONS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 SUBPROGRAM_DECLARATIONS` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 SUBPROGRAM_DECLARATION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 SUBPROGRAM_DECLARATION^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 SUBPROGRAM_DECLARATION^^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 SUBPROGRAM_HEAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 SUBPROGRAM_HEAD^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 ARGUMENTS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 PARAMETER_LIST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 PARAMETER_LIST` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 COMPOUND_STATEMENT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 COMPOUND_STATEMENT^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 OPTIONAL_STATEMENTS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 STATEMENT_LIST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 STATEMENT_LIST` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 STATEMENT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 STATEMENT^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 VARIABLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 VARIABLE^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 PROCEDURE_STATEMENT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 PROCEDURE_STATEMENT^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 EXPRESSION_LIST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 EXPRESSION_LIST` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 EXPRESSION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 EXPRESSION^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 SIMPLE_EXPRESSION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 SIMPLE_EXPRESSION' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 TERM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 TERM` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 FACTOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 FACTOR^ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 SIGN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> program id ( IDENTIFIER_LIST ) ; PROGRAM^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DECLARATIONS PROGRAM^^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COMPOUND_STATEMENT .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id IDENTIFIER_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> , id IDENTIFIER_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> var id : TYPE ; DECLARATIONS`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> var id : TYPE ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STANDARD_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> array [ num .. num ] of STANDARD_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> real</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBPROGRAM_DECLARATION ; SUBPROGRAM_DECLARATIONS`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBPROGRAM_HEAD SUBPROGRAM_DECLARATION^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DECLARATIONS SUBPROGRAM_DECLARATION^^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COMPOUND_STATEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> procedure id SUBPROGRAM_HEAD^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARGUMENTS ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( PARAMETER_LIST )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id : TYPE PARAMETER_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ; id : TYPE PARAMETER_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> begin COMPOUND_STATEMENT^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OPTIONAL_STATEMENTS end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STATEMENT_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STATEMENT STATEMENT_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ; STATEMENT STATEMENT_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VARIABLE assignop EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PROCEDURE_STATEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if EXPRESSION then STATEMENT STATEMENT^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> while EXPRESSION do STATEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> else STATEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id VARIABLE^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ EXPRESSION ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> call id PROCEDURE_STATEMENT^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( EXPRESSION_LIST )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> , EXPRESSION EXPRESSION_LIST`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relop SIMPLE_EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TERM SIMPLE_EXPRESSION`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SIGN TERM SIMPLE_EXPRESSION`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> addop TERM SIMPLE_EXPRESSION`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FACTOR TERM`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mulop FACTOR TERM`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id FACTOR^</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> num</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( EXPRESSION )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> not FACTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,6 +780,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,8 +817,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -520,7 +898,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -551,6 +929,11 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -581,6 +964,11 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,6 +982,10 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="copyForImport" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,48 +1310,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
+    </sheetView>
+    <sheetView topLeftCell="A2" workbookViewId="1">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:42">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="W1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:42">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="V2" s="1" t="str">
+        <f>G!B1</f>
+        <v xml:space="preserve"> program id ( IDENTIFIER_LIST ) ; PROGRAM^</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="1" t="str">
+        <f>G!B2</f>
+        <v xml:space="preserve"> DECLARATIONS PROGRAM^^</v>
+      </c>
+      <c r="AB3" s="1" t="str">
+        <f>G!B3</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
+      </c>
+      <c r="AC3" s="1" t="str">
+        <f>G!B4</f>
+        <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="1" t="str">
+        <f>G!B5</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
+      </c>
+      <c r="AC4" s="1" t="str">
+        <f>G!B6</f>
+        <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AP5" s="1" t="str">
+        <f>G!B7</f>
+        <v xml:space="preserve"> id IDENTIFIER_LIST`</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42">
+      <c r="A6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:42">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42">
+      <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="A15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -971,7 +1705,10 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="F57" sqref="F57"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="1">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2242,10 +2979,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2256,8 +2995,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2278,7 +3020,7 @@
         <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2344,7 +3086,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2355,7 +3097,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2366,7 +3108,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2377,7 +3119,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2443,7 +3185,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2454,7 +3196,7 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2498,7 +3240,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2509,7 +3251,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2553,7 +3295,7 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2564,7 +3306,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2597,7 +3339,7 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2608,7 +3350,7 @@
         <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2619,7 +3361,7 @@
         <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2641,7 +3383,7 @@
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2652,7 +3394,7 @@
         <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2663,7 +3405,7 @@
         <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2674,7 +3416,7 @@
         <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2685,7 +3427,7 @@
         <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2696,7 +3438,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2707,7 +3449,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2718,7 +3460,7 @@
         <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2738,6 +3480,617 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
making progress filling out parse table
despite kitten trying to distract me
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17500" windowHeight="17480" tabRatio="500"/>
-    <workbookView xWindow="17720" yWindow="0" windowWidth="11080" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="39700" windowHeight="16960" tabRatio="500"/>
+    <workbookView xWindow="39820" yWindow="0" windowWidth="11380" windowHeight="31480" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
     <sheet name="firsts" sheetId="2" r:id="rId2"/>
     <sheet name="Follows" sheetId="4" r:id="rId3"/>
-    <sheet name="G" sheetId="7" r:id="rId4"/>
+    <sheet name="Gr" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="1">firsts!$A$2:$J$74</definedName>
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="2">Follows!$A$2:$G$42</definedName>
-    <definedName name="copyForImport" localSheetId="3">G!$A$1:$B$73</definedName>
+    <definedName name="copyForImport" localSheetId="3">Gr!$A$1:$B$73</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -55,7 +55,7 @@
     </textPr>
   </connection>
   <connection id="3" name="copyForImport" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="ENTERPRISE:Users:kuxhausen:Desktop:compiler-front-end:doc:copyForImport" tab="0" qualifier="none" delimiter="@">
+    <textPr fileType="mac" sourceFile="ENTERPRISE:Users:kuxhausen:Desktop:compiler-front-end:doc:copyForImport" tab="0" qualifier="none" delimiter="@">
       <textFields count="2">
         <textField type="text"/>
         <textField type="text"/>
@@ -890,13 +890,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1312,11 +1314,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
+      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
     </sheetView>
     <sheetView topLeftCell="A2" workbookViewId="1">
       <selection activeCell="A3" sqref="A3"/>
@@ -1325,130 +1327,139 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="10.83203125" style="4"/>
+    <col min="22" max="22" width="37.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" style="4"/>
+    <col min="26" max="27" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="49.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="42" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42">
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1456,8 +1467,8 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f>G!B1</f>
+      <c r="V2" s="4" t="str">
+        <f>Gr!B1</f>
         <v xml:space="preserve"> program id ( IDENTIFIER_LIST ) ; PROGRAM^</v>
       </c>
     </row>
@@ -1466,15 +1477,15 @@
         <v>7</v>
       </c>
       <c r="W3" s="1" t="str">
-        <f>G!B2</f>
+        <f>Gr!B2</f>
         <v xml:space="preserve"> DECLARATIONS PROGRAM^^</v>
       </c>
-      <c r="AB3" s="1" t="str">
-        <f>G!B3</f>
+      <c r="AB3" s="4" t="str">
+        <f>Gr!B3</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
       </c>
-      <c r="AC3" s="1" t="str">
-        <f>G!B4</f>
+      <c r="AC3" s="4" t="str">
+        <f>Gr!B4</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
@@ -1482,12 +1493,12 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AB4" s="1" t="str">
-        <f>G!B5</f>
+      <c r="AB4" s="4" t="str">
+        <f>Gr!B5</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
       </c>
-      <c r="AC4" s="1" t="str">
-        <f>G!B6</f>
+      <c r="AC4" s="4" t="str">
+        <f>Gr!B6</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
@@ -1495,8 +1506,8 @@
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AP5" s="1" t="str">
-        <f>G!B7</f>
+      <c r="AP5" s="4" t="str">
+        <f>Gr!B7</f>
         <v xml:space="preserve"> id IDENTIFIER_LIST`</v>
       </c>
     </row>
@@ -1504,27 +1515,61 @@
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="1" t="str">
+        <f>Gr!B9</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f>Gr!B8</f>
+        <v xml:space="preserve"> , id IDENTIFIER_LIST`</v>
+      </c>
     </row>
     <row r="7" spans="1:42">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="W7" s="1" t="str">
+        <f>Gr!B10</f>
+        <v xml:space="preserve"> var id : TYPE ; DECLARATIONS`</v>
+      </c>
     </row>
     <row r="8" spans="1:42">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W8" s="1" t="str">
+        <f>Gr!B11</f>
+        <v xml:space="preserve"> var id : TYPE ;</v>
+      </c>
+      <c r="AB8" s="1" t="str">
+        <f>Gr!B12</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AC8" s="1" t="str">
+        <f>Gr!B12</f>
+        <v xml:space="preserve"> e</v>
+      </c>
     </row>
     <row r="9" spans="1:42">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="Z9" s="1" t="str">
+        <f>Gr!B13</f>
+        <v xml:space="preserve"> STANDARD_TYPE</v>
+      </c>
+      <c r="AA9" s="1" t="str">
+        <f>Gr!B13</f>
+        <v xml:space="preserve"> STANDARD_TYPE</v>
+      </c>
     </row>
     <row r="10" spans="1:42">
       <c r="A10" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f>Gr!B14</f>
+        <v xml:space="preserve"> array [ num .. num ] of STANDARD_TYPE</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -1707,8 +1752,8 @@
     <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="1">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2999,7 +3044,7 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
significant progress on the parse table
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="39700" windowHeight="16960" tabRatio="500"/>
-    <workbookView xWindow="39820" yWindow="0" windowWidth="11380" windowHeight="31480" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="39700" windowHeight="17140" tabRatio="500"/>
+    <workbookView xWindow="39820" yWindow="0" windowWidth="11380" windowHeight="31560" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="228">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t xml:space="preserve"> not FACTOR</t>
+  </si>
+  <si>
+    <t>=Gr!B45 +"|" + =Gr!B46</t>
   </si>
 </sst>
 </file>
@@ -1312,13 +1315,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP42"/>
+  <dimension ref="A1:AQ42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomRight" activeCell="AK32" sqref="AK32"/>
     </sheetView>
     <sheetView topLeftCell="A2" workbookViewId="1">
       <selection activeCell="A3" sqref="A3"/>
@@ -1327,18 +1330,35 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="27.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="21" width="10.83203125" style="4"/>
     <col min="22" max="22" width="37.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.83203125" style="4"/>
     <col min="26" max="27" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="49.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="42" width="10.83203125" style="4"/>
+    <col min="28" max="28" width="53.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" style="4"/>
+    <col min="31" max="31" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.83203125" style="4"/>
+    <col min="33" max="33" width="20.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.83203125" style="4"/>
+    <col min="36" max="36" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="10.83203125" style="4"/>
+    <col min="42" max="42" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:43">
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1462,8 +1482,11 @@
       <c r="AP1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:42">
+      <c r="AQ1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1495,7 @@
         <v xml:space="preserve"> program id ( IDENTIFIER_LIST ) ; PROGRAM^</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:43">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1512,7 @@
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:43">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1502,7 +1525,7 @@
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:43">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1511,7 +1534,7 @@
         <v xml:space="preserve"> id IDENTIFIER_LIST`</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:43">
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
@@ -1524,7 +1547,7 @@
         <v xml:space="preserve"> , id IDENTIFIER_LIST`</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:43">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1533,7 +1556,7 @@
         <v xml:space="preserve"> var id : TYPE ; DECLARATIONS`</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:43">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1550,9 +1573,13 @@
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:43">
       <c r="A9" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f>Gr!B14</f>
+        <v xml:space="preserve"> array [ num .. num ] of STANDARD_TYPE</v>
       </c>
       <c r="Z9" s="1" t="str">
         <f>Gr!B13</f>
@@ -1563,123 +1590,352 @@
         <v xml:space="preserve"> STANDARD_TYPE</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:43">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X10" s="1" t="str">
-        <f>Gr!B14</f>
-        <v xml:space="preserve"> array [ num .. num ] of STANDARD_TYPE</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42">
+      <c r="X10" s="1"/>
+      <c r="Z10" s="1" t="str">
+        <f>Gr!B15</f>
+        <v xml:space="preserve"> integer</v>
+      </c>
+      <c r="AA10" s="1" t="str">
+        <f>Gr!B16</f>
+        <v xml:space="preserve"> real</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:42">
+      <c r="AB11" s="1" t="str">
+        <f>Gr!B17</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATION ; SUBPROGRAM_DECLARATIONS`</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:42">
+      <c r="AB12" s="1" t="str">
+        <f>Gr!B18</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATION ; SUBPROGRAM_DECLARATIONS`</v>
+      </c>
+      <c r="AC12" s="1" t="str">
+        <f>Gr!B19</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:42">
+      <c r="AB13" s="1" t="str">
+        <f>Gr!B20</f>
+        <v xml:space="preserve"> SUBPROGRAM_HEAD SUBPROGRAM_DECLARATION^</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:42">
+      <c r="W14" s="1" t="str">
+        <f>Gr!B21</f>
+        <v xml:space="preserve"> DECLARATIONS SUBPROGRAM_DECLARATION^^</v>
+      </c>
+      <c r="AB14" s="1" t="str">
+        <f>Gr!B22</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT</v>
+      </c>
+      <c r="AC14" s="1" t="str">
+        <f>Gr!B23</f>
+        <v xml:space="preserve"> COMPOUND_STATEMENT</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:42">
+      <c r="AB15" s="1" t="str">
+        <f>Gr!B24</f>
+        <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT</v>
+      </c>
+      <c r="AC15" s="1" t="str">
+        <f>Gr!B25</f>
+        <v xml:space="preserve"> COMPOUND_STATEMENT</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="1"/>
+      <c r="AB16" s="1" t="str">
+        <f>Gr!B26</f>
+        <v xml:space="preserve"> procedure id SUBPROGRAM_HEAD^</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="str">
+        <f>Gr!B27</f>
+        <v xml:space="preserve"> ARGUMENTS ;</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>Gr!B28</f>
+        <v xml:space="preserve"> ;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="1" t="str">
+        <f>Gr!B29</f>
+        <v xml:space="preserve"> ( PARAMETER_LIST )</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="AP19" s="1" t="str">
+        <f>Gr!B30</f>
+        <v xml:space="preserve"> id : TYPE PARAMETER_LIST`</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="C20" s="1" t="str">
+        <f>Gr!B32</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>Gr!B31</f>
+        <v xml:space="preserve"> ; id : TYPE PARAMETER_LIST`</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="AC21" s="1" t="str">
+        <f>Gr!B33</f>
+        <v xml:space="preserve"> begin COMPOUND_STATEMENT^</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="AC22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+      <c r="AD22" s="1" t="str">
+        <f>Gr!B35</f>
+        <v xml:space="preserve"> end</v>
+      </c>
+      <c r="AE22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+      <c r="AH22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+      <c r="AJ22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+      <c r="AP22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="AC23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+      <c r="AE23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+      <c r="AH23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+      <c r="AJ23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+      <c r="AP23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="AC24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AE24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AH24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AJ24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AP24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="D25" s="1" t="str">
+        <f>Gr!B38</f>
+        <v xml:space="preserve"> ; STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AD25" s="1" t="str">
+        <f>Gr!B39</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43">
       <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="AC26" s="1" t="str">
+        <f>Gr!B42</f>
+        <v xml:space="preserve"> COMPOUND_STATEMENT</v>
+      </c>
+      <c r="AE26" s="1" t="str">
+        <f>Gr!B43</f>
+        <v xml:space="preserve"> if EXPRESSION then STATEMENT STATEMENT^</v>
+      </c>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1" t="str">
+        <f>Gr!B44</f>
+        <v xml:space="preserve"> while EXPRESSION do STATEMENT</v>
+      </c>
+      <c r="AJ26" s="1" t="str">
+        <f>Gr!B41</f>
+        <v xml:space="preserve"> PROCEDURE_STATEMENT</v>
+      </c>
+      <c r="AP26" s="1" t="str">
+        <f>Gr!B40</f>
+        <v xml:space="preserve"> VARIABLE assignop EXPRESSION</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="D27" s="1" t="str">
+        <f>Gr!B46</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AD27" s="1" t="str">
+        <f>Gr!B46</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="AP28" s="1" t="str">
+        <f>Gr!B47</f>
+        <v xml:space="preserve"> id VARIABLE^</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="H29" s="1" t="str">
+        <f>Gr!B48</f>
+        <v xml:space="preserve"> [ EXPRESSION ]</v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f>Gr!B49</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="AJ30" s="1" t="str">
+        <f>Gr!B50</f>
+        <v xml:space="preserve"> call id PROCEDURE_STATEMENT^</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43">
       <c r="A31" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="1" t="str">
+        <f>Gr!B51</f>
+        <v xml:space="preserve"> ( EXPRESSION_LIST )</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f>Gr!B52</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AD31" s="1" t="str">
+        <f>Gr!B52</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AG31" s="1" t="str">
+        <f>Gr!B52</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43">
       <c r="A32" s="3" t="s">
         <v>69</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AK32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="AP32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="AQ32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -1753,7 +2009,7 @@
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3044,7 +3300,7 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
further parse table progress
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="39700" windowHeight="17140" tabRatio="500"/>
-    <workbookView xWindow="39820" yWindow="0" windowWidth="11380" windowHeight="31560" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="39820" yWindow="-20" windowWidth="11380" windowHeight="31540" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="222">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -435,24 +435,6 @@
   </si>
   <si>
     <t>]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =</t>
-  </si>
-  <si>
-    <t>&lt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>&lt;=</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t>&gt;</t>
   </si>
   <si>
     <t xml:space="preserve"> -</t>
@@ -820,8 +802,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -903,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -939,6 +929,10 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -974,6 +968,10 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1315,13 +1313,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ42"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK32" sqref="AK32"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
     <sheetView topLeftCell="A2" workbookViewId="1">
       <selection activeCell="A3" sqref="A3"/>
@@ -1330,35 +1328,39 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="4"/>
     <col min="4" max="4" width="27.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="4"/>
     <col min="8" max="8" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="21" width="10.83203125" style="4"/>
-    <col min="22" max="22" width="37.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" style="4"/>
-    <col min="26" max="27" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="53.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.83203125" style="4"/>
-    <col min="31" max="31" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.83203125" style="4"/>
-    <col min="33" max="33" width="20.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.83203125" style="4"/>
-    <col min="36" max="36" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="41" width="10.83203125" style="4"/>
-    <col min="42" max="42" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="4"/>
+    <col min="12" max="13" width="30.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.83203125" style="4"/>
+    <col min="16" max="16" width="37.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="4"/>
+    <col min="20" max="21" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="53.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="4"/>
+    <col min="25" max="25" width="39.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.83203125" style="4"/>
+    <col min="27" max="27" width="20.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" style="4"/>
+    <col min="30" max="30" width="28.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.83203125" style="4"/>
+    <col min="36" max="36" width="30.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:39">
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1390,10 +1392,10 @@
         <v>57</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>125</v>
@@ -1401,140 +1403,128 @@
       <c r="O1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>132</v>
+      <c r="P1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AJ1" s="5" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="AK1" s="5" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="4" t="str">
+      <c r="P2" s="4" t="str">
         <f>Gr!B1</f>
         <v xml:space="preserve"> program id ( IDENTIFIER_LIST ) ; PROGRAM^</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:39">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="1" t="str">
+      <c r="Q3" s="1" t="str">
         <f>Gr!B2</f>
         <v xml:space="preserve"> DECLARATIONS PROGRAM^^</v>
       </c>
-      <c r="AB3" s="4" t="str">
+      <c r="V3" s="4" t="str">
         <f>Gr!B3</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
       </c>
-      <c r="AC3" s="4" t="str">
+      <c r="W3" s="4" t="str">
         <f>Gr!B4</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:39">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AB4" s="4" t="str">
+      <c r="V4" s="4" t="str">
         <f>Gr!B5</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT .</v>
       </c>
-      <c r="AC4" s="4" t="str">
+      <c r="W4" s="4" t="str">
         <f>Gr!B6</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT .</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:39">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AP5" s="4" t="str">
+      <c r="AJ5" s="4" t="str">
         <f>Gr!B7</f>
         <v xml:space="preserve"> id IDENTIFIER_LIST`</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:39">
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
@@ -1547,135 +1537,135 @@
         <v xml:space="preserve"> , id IDENTIFIER_LIST`</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:39">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="1" t="str">
+      <c r="Q7" s="1" t="str">
         <f>Gr!B10</f>
         <v xml:space="preserve"> var id : TYPE ; DECLARATIONS`</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:39">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W8" s="1" t="str">
+      <c r="Q8" s="1" t="str">
         <f>Gr!B11</f>
         <v xml:space="preserve"> var id : TYPE ;</v>
       </c>
-      <c r="AB8" s="1" t="str">
+      <c r="V8" s="1" t="str">
         <f>Gr!B12</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AC8" s="1" t="str">
+      <c r="W8" s="1" t="str">
         <f>Gr!B12</f>
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:39">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X9" s="1" t="str">
+      <c r="R9" s="1" t="str">
         <f>Gr!B14</f>
         <v xml:space="preserve"> array [ num .. num ] of STANDARD_TYPE</v>
       </c>
-      <c r="Z9" s="1" t="str">
+      <c r="T9" s="1" t="str">
         <f>Gr!B13</f>
         <v xml:space="preserve"> STANDARD_TYPE</v>
       </c>
-      <c r="AA9" s="1" t="str">
+      <c r="U9" s="1" t="str">
         <f>Gr!B13</f>
         <v xml:space="preserve"> STANDARD_TYPE</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:39">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X10" s="1"/>
-      <c r="Z10" s="1" t="str">
+      <c r="R10" s="1"/>
+      <c r="T10" s="1" t="str">
         <f>Gr!B15</f>
         <v xml:space="preserve"> integer</v>
       </c>
-      <c r="AA10" s="1" t="str">
+      <c r="U10" s="1" t="str">
         <f>Gr!B16</f>
         <v xml:space="preserve"> real</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:39">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AB11" s="1" t="str">
+      <c r="V11" s="1" t="str">
         <f>Gr!B17</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATION ; SUBPROGRAM_DECLARATIONS`</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:39">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AB12" s="1" t="str">
+      <c r="V12" s="1" t="str">
         <f>Gr!B18</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATION ; SUBPROGRAM_DECLARATIONS`</v>
       </c>
-      <c r="AC12" s="1" t="str">
+      <c r="W12" s="1" t="str">
         <f>Gr!B19</f>
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:39">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AB13" s="1" t="str">
+      <c r="V13" s="1" t="str">
         <f>Gr!B20</f>
         <v xml:space="preserve"> SUBPROGRAM_HEAD SUBPROGRAM_DECLARATION^</v>
       </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:39">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="W14" s="1" t="str">
+      <c r="Q14" s="1" t="str">
         <f>Gr!B21</f>
         <v xml:space="preserve"> DECLARATIONS SUBPROGRAM_DECLARATION^^</v>
       </c>
-      <c r="AB14" s="1" t="str">
+      <c r="V14" s="1" t="str">
         <f>Gr!B22</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT</v>
       </c>
-      <c r="AC14" s="1" t="str">
+      <c r="W14" s="1" t="str">
         <f>Gr!B23</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT</v>
       </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:39">
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AB15" s="1" t="str">
+      <c r="V15" s="1" t="str">
         <f>Gr!B24</f>
         <v xml:space="preserve"> SUBPROGRAM_DECLARATIONS COMPOUND_STATEMENT</v>
       </c>
-      <c r="AC15" s="1" t="str">
+      <c r="W15" s="1" t="str">
         <f>Gr!B25</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:39">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="AB16" s="1" t="str">
+      <c r="V16" s="1" t="str">
         <f>Gr!B26</f>
         <v xml:space="preserve"> procedure id SUBPROGRAM_HEAD^</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:37">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1688,7 +1678,7 @@
         <v xml:space="preserve"> ;</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:37">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
@@ -1697,16 +1687,16 @@
         <v xml:space="preserve"> ( PARAMETER_LIST )</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:37">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AP19" s="1" t="str">
+      <c r="AJ19" s="1" t="str">
         <f>Gr!B30</f>
         <v xml:space="preserve"> id : TYPE PARAMETER_LIST`</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:37">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1719,32 +1709,36 @@
         <v xml:space="preserve"> ; id : TYPE PARAMETER_LIST`</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:37">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AC21" s="1" t="str">
+      <c r="W21" s="1" t="str">
         <f>Gr!B33</f>
         <v xml:space="preserve"> begin COMPOUND_STATEMENT^</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:37">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC22" s="1" t="str">
+      <c r="W22" s="1" t="str">
         <f>Gr!B34</f>
         <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
       </c>
-      <c r="AD22" s="1" t="str">
+      <c r="X22" s="1" t="str">
         <f>Gr!B35</f>
         <v xml:space="preserve"> end</v>
       </c>
-      <c r="AE22" s="1" t="str">
+      <c r="Y22" s="1" t="str">
         <f>Gr!B34</f>
         <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
       </c>
-      <c r="AH22" s="1" t="str">
+      <c r="AB22" s="1" t="str">
+        <f>Gr!B34</f>
+        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
+      </c>
+      <c r="AD22" s="1" t="str">
         <f>Gr!B34</f>
         <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
       </c>
@@ -1752,24 +1746,24 @@
         <f>Gr!B34</f>
         <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
       </c>
-      <c r="AP22" s="1" t="str">
-        <f>Gr!B34</f>
-        <v xml:space="preserve"> OPTIONAL_STATEMENTS end</v>
-      </c>
-    </row>
-    <row r="23" spans="1:43">
+    </row>
+    <row r="23" spans="1:37">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AC23" s="1" t="str">
+      <c r="W23" s="1" t="str">
         <f>Gr!B36</f>
         <v xml:space="preserve"> STATEMENT_LIST</v>
       </c>
-      <c r="AE23" s="1" t="str">
+      <c r="Y23" s="1" t="str">
         <f>Gr!B36</f>
         <v xml:space="preserve"> STATEMENT_LIST</v>
       </c>
-      <c r="AH23" s="1" t="str">
+      <c r="AB23" s="1" t="str">
+        <f>Gr!B36</f>
+        <v xml:space="preserve"> STATEMENT_LIST</v>
+      </c>
+      <c r="AD23" s="1" t="str">
         <f>Gr!B36</f>
         <v xml:space="preserve"> STATEMENT_LIST</v>
       </c>
@@ -1777,24 +1771,24 @@
         <f>Gr!B36</f>
         <v xml:space="preserve"> STATEMENT_LIST</v>
       </c>
-      <c r="AP23" s="1" t="str">
-        <f>Gr!B36</f>
-        <v xml:space="preserve"> STATEMENT_LIST</v>
-      </c>
-    </row>
-    <row r="24" spans="1:43">
+    </row>
+    <row r="24" spans="1:37">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AC24" s="1" t="str">
+      <c r="W24" s="1" t="str">
         <f>Gr!B37</f>
         <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
       </c>
-      <c r="AE24" s="1" t="str">
+      <c r="Y24" s="1" t="str">
         <f>Gr!B37</f>
         <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
       </c>
-      <c r="AH24" s="1" t="str">
+      <c r="AB24" s="1" t="str">
+        <f>Gr!B37</f>
+        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
+      </c>
+      <c r="AD24" s="1" t="str">
         <f>Gr!B37</f>
         <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
       </c>
@@ -1802,12 +1796,8 @@
         <f>Gr!B37</f>
         <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
       </c>
-      <c r="AP24" s="1" t="str">
-        <f>Gr!B37</f>
-        <v xml:space="preserve"> STATEMENT STATEMENT_LIST`</v>
-      </c>
-    </row>
-    <row r="25" spans="1:43">
+    </row>
+    <row r="25" spans="1:37">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -1815,38 +1805,38 @@
         <f>Gr!B38</f>
         <v xml:space="preserve"> ; STATEMENT STATEMENT_LIST`</v>
       </c>
-      <c r="AD25" s="1" t="str">
+      <c r="X25" s="1" t="str">
         <f>Gr!B39</f>
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:37">
       <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AC26" s="1" t="str">
+      <c r="W26" s="1" t="str">
         <f>Gr!B42</f>
         <v xml:space="preserve"> COMPOUND_STATEMENT</v>
       </c>
-      <c r="AE26" s="1" t="str">
+      <c r="Y26" s="1" t="str">
         <f>Gr!B43</f>
         <v xml:space="preserve"> if EXPRESSION then STATEMENT STATEMENT^</v>
       </c>
-      <c r="AG26" s="1"/>
-      <c r="AH26" s="1" t="str">
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1" t="str">
         <f>Gr!B44</f>
         <v xml:space="preserve"> while EXPRESSION do STATEMENT</v>
       </c>
-      <c r="AJ26" s="1" t="str">
+      <c r="AD26" s="1" t="str">
         <f>Gr!B41</f>
         <v xml:space="preserve"> PROCEDURE_STATEMENT</v>
       </c>
-      <c r="AP26" s="1" t="str">
+      <c r="AJ26" s="1" t="str">
         <f>Gr!B40</f>
         <v xml:space="preserve"> VARIABLE assignop EXPRESSION</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:37">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1854,24 +1844,24 @@
         <f>Gr!B46</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AD27" s="1" t="str">
+      <c r="X27" s="1" t="str">
         <f>Gr!B46</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AG27" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:43">
+      <c r="AA27" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AP28" s="1" t="str">
+      <c r="AJ28" s="1" t="str">
         <f>Gr!B47</f>
         <v xml:space="preserve"> id VARIABLE^</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:37">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -1884,16 +1874,16 @@
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:37">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AJ30" s="1" t="str">
+      <c r="AD30" s="1" t="str">
         <f>Gr!B50</f>
         <v xml:space="preserve"> call id PROCEDURE_STATEMENT^</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:37">
       <c r="A31" s="3" t="s">
         <v>68</v>
       </c>
@@ -1905,16 +1895,16 @@
         <f>Gr!B52</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AD31" s="1" t="str">
+      <c r="X31" s="1" t="str">
         <f>Gr!B52</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AG31" s="1" t="str">
+      <c r="AA31" s="1" t="str">
         <f>Gr!B52</f>
         <v xml:space="preserve"> e</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:37">
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
@@ -1923,67 +1913,204 @@
         <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AG32" s="1"/>
+      <c r="L32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="M32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="X32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AE32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+      <c r="AJ32" s="1" t="str">
+        <f>Gr!B53</f>
+        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
+      </c>
       <c r="AK32" s="1" t="str">
         <f>Gr!B53</f>
         <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
       </c>
-      <c r="AP32" s="1" t="str">
-        <f>Gr!B53</f>
-        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
-      </c>
-      <c r="AQ32" s="1" t="str">
-        <f>Gr!B53</f>
-        <v xml:space="preserve"> EXPRESSION EXPRESSION_LIST`</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+    </row>
+    <row r="33" spans="1:39">
       <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="C33" s="1" t="str">
+        <f>Gr!B55</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f>Gr!B54</f>
+        <v xml:space="preserve"> , EXPRESSION EXPRESSION_LIST`</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39">
       <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+      <c r="L34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+      <c r="M34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+      <c r="AE34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+      <c r="AJ34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+      <c r="AK34" s="1" t="str">
+        <f>Gr!B56</f>
+        <v xml:space="preserve"> SIMPLE_EXPRESSION EXPRESSION^</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
       <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="C35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="X35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="Z35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AA35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AC35" s="1" t="str">
+        <f>Gr!B58</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AL35" s="1" t="str">
+        <f>Gr!B57</f>
+        <v xml:space="preserve"> relop SIMPLE_EXPRESSION</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
       <c r="A36" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="1" t="str">
+        <f>Gr!B59</f>
+        <v xml:space="preserve"> TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="L36" s="1" t="str">
+        <f>Gr!B60</f>
+        <v xml:space="preserve"> SIGN TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="M36" s="1" t="str">
+        <f>Gr!B60</f>
+        <v xml:space="preserve"> SIGN TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="AE36" s="1" t="str">
+        <f>Gr!B59</f>
+        <v xml:space="preserve"> TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="AJ36" s="1" t="str">
+        <f>Gr!B59</f>
+        <v xml:space="preserve"> TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="AK36" s="1" t="str">
+        <f>Gr!B59</f>
+        <v xml:space="preserve"> TERM SIMPLE_EXPRESSION`</v>
+      </c>
+      <c r="AM36" s="4"/>
+    </row>
+    <row r="37" spans="1:39">
       <c r="A37" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="C37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="J37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="X37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="Z37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AA37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AC37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AL37" s="1" t="str">
+        <f>Gr!B62</f>
+        <v xml:space="preserve"> e</v>
+      </c>
+      <c r="AM37" s="1" t="str">
+        <f>Gr!B61</f>
+        <v xml:space="preserve"> addop TERM SIMPLE_EXPRESSION`</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
       <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:39">
       <c r="A39" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:39">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:39">
       <c r="A41" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:39">
       <c r="A42" s="3" t="s">
         <v>78</v>
       </c>
@@ -2008,8 +2135,8 @@
     <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3299,8 +3426,8 @@
     <sheetView topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3387,7 +3514,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3398,7 +3525,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3804,586 +3931,586 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved dangling else ambiguity in parse table
Resolved by removing entry for “if EXPRESSION then STATEMENT” so that
only “if EXPRESSION then STATEMENT else STATEMENT” is valid
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="39700" windowHeight="17140" tabRatio="500"/>
-    <workbookView xWindow="39820" yWindow="-20" windowWidth="11380" windowHeight="31540" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="40380" yWindow="-20" windowWidth="10820" windowHeight="31540" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40180" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="217">
   <si>
     <t>PROGRAM</t>
   </si>
@@ -717,9 +717,6 @@
   </si>
   <si>
     <t xml:space="preserve"> not FACTOR</t>
-  </si>
-  <si>
-    <t>=Gr!B45 +"|" + =Gr!B46</t>
   </si>
 </sst>
 </file>
@@ -1303,14 +1300,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="M42" sqref="M42"/>
     </sheetView>
-    <sheetView topLeftCell="A2" workbookViewId="1">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1826,8 +1826,9 @@
         <f>Gr!B46</f>
         <v xml:space="preserve"> e</v>
       </c>
-      <c r="AA27" s="1" t="s">
-        <v>217</v>
+      <c r="AA27" s="1" t="str">
+        <f>Gr!B45</f>
+        <v xml:space="preserve"> else STATEMENT</v>
       </c>
     </row>
     <row r="28" spans="1:33">
@@ -2247,11 +2248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3538,8 +3539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C35" sqref="C35"/>

</xml_diff>

<commit_message>
fixed bug in DeclarationsTail production in grammar
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="-20" windowWidth="10820" windowHeight="31540" tabRatio="500" firstSheet="1" activeTab="1"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40180" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="51200" windowHeight="32000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -587,9 +586,6 @@
     <t xml:space="preserve"> var id : TYPE ; DECLARATIONS`</t>
   </si>
   <si>
-    <t xml:space="preserve"> var id : TYPE ;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> STANDARD_TYPE</t>
   </si>
   <si>
@@ -717,6 +713,9 @@
   </si>
   <si>
     <t xml:space="preserve"> not FACTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> var id : TYPE ;  DECLARATIONS`</t>
   </si>
 </sst>
 </file>
@@ -1301,16 +1300,10 @@
   <dimension ref="A1:AJ42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M42" sqref="M42"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA27" sqref="AA27"/>
+      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1530,7 +1523,7 @@
       </c>
       <c r="Q8" s="1" t="str">
         <f>Gr!B11</f>
-        <v xml:space="preserve"> var id : TYPE ;</v>
+        <v xml:space="preserve"> var id : TYPE ;  DECLARATIONS`</v>
       </c>
       <c r="V8" s="1" t="str">
         <f>Gr!B12</f>
@@ -2237,7 +2230,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2248,11 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3529,7 +3518,6 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -3540,10 +3528,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4024,7 +4009,6 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -4034,10 +4018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -4130,7 +4113,7 @@
         <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4146,7 +4129,7 @@
         <v>131</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4154,7 +4137,7 @@
         <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4162,7 +4145,7 @@
         <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4170,7 +4153,7 @@
         <v>132</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4178,7 +4161,7 @@
         <v>133</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4186,7 +4169,7 @@
         <v>134</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4202,7 +4185,7 @@
         <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4210,7 +4193,7 @@
         <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4218,7 +4201,7 @@
         <v>136</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4226,7 +4209,7 @@
         <v>136</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4234,7 +4217,7 @@
         <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4242,7 +4225,7 @@
         <v>137</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4250,7 +4233,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4258,7 +4241,7 @@
         <v>139</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4266,7 +4249,7 @@
         <v>139</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4274,7 +4257,7 @@
         <v>140</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4282,7 +4265,7 @@
         <v>141</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4290,7 +4273,7 @@
         <v>142</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4306,7 +4289,7 @@
         <v>143</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4314,7 +4297,7 @@
         <v>144</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4322,7 +4305,7 @@
         <v>144</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4330,7 +4313,7 @@
         <v>145</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4338,7 +4321,7 @@
         <v>146</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4346,7 +4329,7 @@
         <v>147</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4362,7 +4345,7 @@
         <v>148</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4370,7 +4353,7 @@
         <v>148</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4378,7 +4361,7 @@
         <v>148</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4386,7 +4369,7 @@
         <v>148</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4394,7 +4377,7 @@
         <v>148</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4402,7 +4385,7 @@
         <v>149</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4418,7 +4401,7 @@
         <v>150</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4426,7 +4409,7 @@
         <v>151</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4442,7 +4425,7 @@
         <v>152</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4450,7 +4433,7 @@
         <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4466,7 +4449,7 @@
         <v>154</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4474,7 +4457,7 @@
         <v>155</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4490,7 +4473,7 @@
         <v>156</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4498,7 +4481,7 @@
         <v>157</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4514,7 +4497,7 @@
         <v>158</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4522,7 +4505,7 @@
         <v>158</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4530,7 +4513,7 @@
         <v>159</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4546,7 +4529,7 @@
         <v>160</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4554,7 +4537,7 @@
         <v>161</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4570,7 +4553,7 @@
         <v>162</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4578,7 +4561,7 @@
         <v>162</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4586,7 +4569,7 @@
         <v>162</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4594,7 +4577,7 @@
         <v>162</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4602,7 +4585,7 @@
         <v>163</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4634,7 +4617,6 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Saved earlier (apparently unsaved) change to parse table
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="51200" windowHeight="32000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -1300,10 +1300,10 @@
   <dimension ref="A1:AJ42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
massive last minute documentation work
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="31480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -786,8 +786,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -877,7 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -917,6 +945,20 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -956,6 +998,20 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2241,16 +2297,16 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection sqref="A1:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -3527,15 +3583,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -4018,7 +4074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improved parse table printing
</commit_message>
<xml_diff>
--- a/doc/ParseTable.xlsx
+++ b/doc/ParseTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="31480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="31480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ParseTable" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="1">firsts!$A$2:$J$74</definedName>
     <definedName name="_2014PascalGrammarSubset_SpecChange_Numbered_NullProdRemoved_LeftRecurRemoved_LeftFactored" localSheetId="2">Follows!$A$2:$G$42</definedName>
     <definedName name="copyForImport" localSheetId="3">Gr!$A$1:$B$73</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">ParseTable!$A:$A,ParseTable!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1355,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2282,11 +2283,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <printOptions headings="1" gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="60"/>
     </ext>
   </extLst>
 </worksheet>
@@ -3583,7 +3585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection sqref="A1:C42"/>
     </sheetView>
   </sheetViews>

</xml_diff>